<commit_message>
Updated build for basic project, separated out some transmission pair-specific logic
</commit_message>
<xml_diff>
--- a/tabular/refseq_data/lanl-alignment-data.xlsx
+++ b/tabular/refseq_data/lanl-alignment-data.xlsx
@@ -17580,13 +17580,13 @@
     <t>Subtype</t>
   </si>
   <si>
-    <t>Country-ISO</t>
-  </si>
-  <si>
     <t>Isolate-name</t>
   </si>
   <si>
     <t>Year</t>
+  </si>
+  <si>
+    <t>Country</t>
   </si>
 </sst>
 </file>
@@ -18008,7 +18008,7 @@
   <dimension ref="A1:E2876"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="H14:I15"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -18027,13 +18027,13 @@
         <v>5852</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>5855</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>5854</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>5853</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>5855</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>5854</v>
       </c>
     </row>
     <row r="2" spans="1:5">

</xml_diff>